<commit_message>
"Made some slight changes to requirements"
</commit_message>
<xml_diff>
--- a/ECE445-Proposal/Requirements-Verification.xlsx
+++ b/ECE445-Proposal/Requirements-Verification.xlsx
@@ -126,22 +126,22 @@
     </r>
   </si>
   <si>
-    <t>Beam divergence must attain a spot size diameter equivelent to 10 cm and must be  span the range of a human chest (2-3 ft) at the following distances:
+    <t>Must be able to achieve 2.5mW of power at source with a wavelength to be determined.</t>
+  </si>
+  <si>
+    <t>Ability to process signal from R.F. receiver and decode it to match the passphrase with its own internal clock to a precision of ± 10 minutes ± 10%.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to generate an encrypted signal containing passphrase that is based on internal Real Time Clock (RTC) with an precision of ± 10 minutes ± 10%. </t>
+  </si>
+  <si>
+    <t>Ability to control laser transmitter to send digital data by alternating the state of the PWM laser pulse at a predefined time period of ~ 50𝜇s.</t>
+  </si>
+  <si>
+    <t>Beam divergence must attain a spot size diameter equivelent to 10 cm and must span the range of a human chest (2-3 ft) at the following distances:
           - Short Range (0-50 m)
           - Medium Range (50-150 m)
           - Long Range (150-300 m)</t>
-  </si>
-  <si>
-    <t>Must be able to achieve 2.5mW of power at source with a wavelength to be determined.</t>
-  </si>
-  <si>
-    <t>Ability to process signal from R.F. receiver and decode it to match the passphrase with its own internal clock to a precision of ± 10 minutes ± 10%.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ability to generate an encrypted signal containing passphrase that is based on internal Real Time Clock (RTC) with an precision of ± 10 minutes ± 10%. </t>
-  </si>
-  <si>
-    <t>Ability to control laser transmitter to send digital data by alternating the state of the PWM laser pulse at a predefined time period of ~ 50𝜇s.</t>
   </si>
 </sst>
 </file>
@@ -527,6 +527,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,6 +554,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -548,26 +566,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,8 +851,8 @@
   </sheetPr>
   <dimension ref="C2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -886,39 +886,39 @@
       </c>
     </row>
     <row r="3" spans="3:8" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="35" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="30">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="3:8" ht="101" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="33"/>
-      <c r="D4" s="31"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="21" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="31">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="3:8" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="33"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="9" t="s">
         <v>10</v>
       </c>
@@ -934,7 +934,7 @@
       </c>
     </row>
     <row r="6" spans="3:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="33"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="9" t="s">
         <v>8</v>
       </c>
@@ -950,35 +950,35 @@
       </c>
     </row>
     <row r="7" spans="3:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="40"/>
-      <c r="D7" s="30" t="s">
+      <c r="C7" s="39"/>
+      <c r="D7" s="35" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="42"/>
+        <v>30</v>
+      </c>
+      <c r="F7" s="33"/>
       <c r="G7" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="30">
+      <c r="H7" s="35">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="3:8" ht="59" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="34"/>
-      <c r="D8" s="41"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="43"/>
       <c r="E8" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="43"/>
+        <v>28</v>
+      </c>
+      <c r="F8" s="34"/>
       <c r="G8" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="41"/>
+      <c r="H8" s="43"/>
     </row>
     <row r="9" spans="3:8" ht="69" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="36" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="19" t="s">
@@ -991,12 +991,12 @@
       <c r="G9" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="32">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="68" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="35"/>
+      <c r="C10" s="41"/>
       <c r="D10" s="9" t="s">
         <v>11</v>
       </c>
@@ -1012,7 +1012,7 @@
       </c>
     </row>
     <row r="11" spans="3:8" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="35"/>
+      <c r="C11" s="41"/>
       <c r="D11" s="9" t="s">
         <v>8</v>
       </c>
@@ -1028,12 +1028,12 @@
       </c>
     </row>
     <row r="12" spans="3:8" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="36"/>
+      <c r="C12" s="42"/>
       <c r="D12" s="18" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="28" t="s">

</xml_diff>